<commit_message>
Updated Fish indicator to 1 = yes (NOT -1)
</commit_message>
<xml_diff>
--- a/data/SURVEY MASTER_README.xlsx
+++ b/data/SURVEY MASTER_README.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Courtney.S.Couch\Documents\GitHub\fish-paste\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tye.kindinger\Desktop\FISH TEAM\fish-paste\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -257,9 +257,6 @@
     <t>Flag to indicate whether calification accretion units (CAUs) were deployed retrived at a site (0=no, -1= yes)</t>
   </si>
   <si>
-    <t>Flag to indicate whether fish survey were conducted at a site (0=no, -1= yes)</t>
-  </si>
-  <si>
     <t>Flag to indicate whether site is classified as an oceanography and climate change site- needs to be revisited (0=no, -1= yes)</t>
   </si>
   <si>
@@ -297,6 +294,9 @@
   </si>
   <si>
     <t>Columns that need to be double checked or removed</t>
+  </si>
+  <si>
+    <t>Flag to indicate whether fish survey were conducted at a site (0=no, 1= yes)</t>
   </si>
 </sst>
 </file>
@@ -663,28 +663,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="119.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="119.6640625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -692,7 +692,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -700,7 +700,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -708,7 +708,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -716,7 +716,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -724,7 +724,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -732,7 +732,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -740,7 +740,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -748,7 +748,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -756,7 +756,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -764,7 +764,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -772,7 +772,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -780,7 +780,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -788,7 +788,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -796,7 +796,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -804,17 +804,17 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -822,7 +822,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -830,7 +830,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -838,7 +838,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -846,7 +846,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -854,7 +854,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -862,7 +862,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -870,19 +870,19 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="6"/>
     </row>
-    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="6"/>
     </row>
-    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -890,7 +890,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -898,7 +898,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -906,7 +906,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -914,7 +914,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -922,7 +922,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -930,7 +930,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -938,7 +938,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -946,102 +946,102 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>35</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>37</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>38</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>39</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>40</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>41</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>42</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>45</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>46</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SURVEY MASTER updated with 2023 Fish REA sites (+ 4 SfM/PQ-only sites)
</commit_message>
<xml_diff>
--- a/data/SURVEY MASTER_README.xlsx
+++ b/data/SURVEY MASTER_README.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>SITEVISITID</t>
   </si>
@@ -297,6 +297,9 @@
   </si>
   <si>
     <t>Flag to indicate whether fish survey were conducted at a site (0=no, 1= yes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TLK - have stopped updating this as of 2023; transitioned to all NA in 2023; use only 'Fish' column.   </t>
   </si>
 </sst>
 </file>
@@ -663,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -880,7 +883,9 @@
       <c r="A27" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="6"/>
+      <c r="B27" s="6" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">

</xml_diff>